<commit_message>
Initial commit + Push
</commit_message>
<xml_diff>
--- a/coco.xlsx
+++ b/coco.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfped\PycharmProjects\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6DC4F1-DA7F-4C48-BAB8-159C91CC7D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C79CC5B-B3A9-4363-923F-7005E057850E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{F223B1E5-81D5-456F-B28C-0128604884DC}"/>
   </bookViews>
@@ -633,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED47F00B-EA73-4214-A337-6D93F6867154}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>

</xml_diff>